<commit_message>
skip mysql test suite
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>TestID</t>
   </si>
@@ -123,6 +123,24 @@
   <si>
     <t>batch_002</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_003</t>
+  </si>
+  <si>
+    <t>批量操作语句3执行</t>
+  </si>
+  <si>
+    <t>batch03</t>
+  </si>
+  <si>
+    <t>batch_sql_03</t>
+  </si>
+  <si>
+    <t>select * from $batch03</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_003.csv</t>
   </si>
 </sst>
 </file>
@@ -495,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -613,6 +631,35 @@
         <v>25</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove skip cases from yaml
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -21,144 +21,145 @@
     <t>TestID</t>
   </si>
   <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Sub_component</t>
+  </si>
+  <si>
+    <t>Table_value_ref</t>
+  </si>
+  <si>
+    <t>Validation_type</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>csv_equals</t>
+  </si>
+  <si>
+    <t>批量操作语句1执行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批量操作语句2执行</t>
+  </si>
+  <si>
+    <t>csv_containsAll</t>
+  </si>
+  <si>
+    <t>batch_sql_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_sql_02</t>
+  </si>
+  <si>
+    <t>Table_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $batch01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_result1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_sql2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_result2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $batch02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batch_sql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_sql1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_001.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_002.csv</t>
+  </si>
+  <si>
+    <t>batchsql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batchsql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_003</t>
+  </si>
+  <si>
+    <t>批量操作语句3执行</t>
+  </si>
+  <si>
+    <t>batch03</t>
+  </si>
+  <si>
+    <t>batch_sql_03</t>
+  </si>
+  <si>
+    <t>select * from $batch03</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_003.csv</t>
+  </si>
+  <si>
+    <t>batch_004</t>
+  </si>
+  <si>
+    <t>批量操作语句4执行</t>
+  </si>
+  <si>
+    <t>batch04</t>
+  </si>
+  <si>
+    <t>batch_sql_04</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_004.csv</t>
+  </si>
+  <si>
+    <t>select account from $batch04 where account&lt;&gt;'6225880178560985'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Testable</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Component</t>
-  </si>
-  <si>
-    <t>Sub_component</t>
-  </si>
-  <si>
-    <t>Table_value_ref</t>
-  </si>
-  <si>
-    <t>Validation_type</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>csv_equals</t>
-  </si>
-  <si>
-    <t>批量操作语句1执行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>批量操作语句2执行</t>
-  </si>
-  <si>
-    <t>csv_containsAll</t>
-  </si>
-  <si>
-    <t>batch_sql_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_sql_02</t>
-  </si>
-  <si>
-    <t>Table_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from $batch01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_result1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_sql2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_result2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from $batch02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Batch_sql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_sql1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_001.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_002.csv</t>
-  </si>
-  <si>
-    <t>batchsql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batchsql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_003</t>
-  </si>
-  <si>
-    <t>批量操作语句3执行</t>
-  </si>
-  <si>
-    <t>batch03</t>
-  </si>
-  <si>
-    <t>batch_sql_03</t>
-  </si>
-  <si>
-    <t>select * from $batch03</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_003.csv</t>
-  </si>
-  <si>
-    <t>batch_004</t>
-  </si>
-  <si>
-    <t>批量操作语句4执行</t>
-  </si>
-  <si>
-    <t>batch04</t>
-  </si>
-  <si>
-    <t>batch_sql_04</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_004.csv</t>
-  </si>
-  <si>
-    <t>select account from $batch04 where account&lt;&gt;'6225880178560985'</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -534,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -559,156 +560,156 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>35</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exchange mysql and dingo case order, add some hash partition dml cases
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
   <si>
     <t>TestID</t>
   </si>
@@ -161,6 +161,43 @@
   <si>
     <t>Testable</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_005</t>
+  </si>
+  <si>
+    <t>批量操作语句5执行</t>
+  </si>
+  <si>
+    <t>batch05</t>
+  </si>
+  <si>
+    <t>batch_sql_05</t>
+  </si>
+  <si>
+    <t>select * from $batch05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_005.csv</t>
+  </si>
+  <si>
+    <t>batch_006</t>
+  </si>
+  <si>
+    <t>批量操作语句6执行</t>
+  </si>
+  <si>
+    <t>batch06</t>
+  </si>
+  <si>
+    <t>batch_sql_06</t>
+  </si>
+  <si>
+    <t>select * from $batch06</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_006.csv</t>
   </si>
 </sst>
 </file>
@@ -533,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -709,6 +746,64 @@
         <v>39</v>
       </c>
       <c r="M5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A7" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M7" s="6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add case about issue that drop table and create same with only primary key type different
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>TestID</t>
   </si>
@@ -198,6 +198,42 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_006.csv</t>
+  </si>
+  <si>
+    <t>batch_007</t>
+  </si>
+  <si>
+    <t>batch_008</t>
+  </si>
+  <si>
+    <t>批量操作语句7执行</t>
+  </si>
+  <si>
+    <t>批量操作语句8执行</t>
+  </si>
+  <si>
+    <t>batch07</t>
+  </si>
+  <si>
+    <t>batch08</t>
+  </si>
+  <si>
+    <t>batch_sql_07</t>
+  </si>
+  <si>
+    <t>batch_sql_08</t>
+  </si>
+  <si>
+    <t>select * from $batch07</t>
+  </si>
+  <si>
+    <t>select * from $batch08</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_007.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_008.csv</t>
   </si>
 </sst>
 </file>
@@ -570,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -804,6 +840,64 @@
         <v>53</v>
       </c>
       <c r="M7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" s="6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add batch sql about nacos
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
   <si>
     <t>TestID</t>
   </si>
@@ -27,213 +27,251 @@
     <t>Component</t>
   </si>
   <si>
+    <t>Table_value_ref</t>
+  </si>
+  <si>
+    <t>Validation_type</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>csv_equals</t>
+  </si>
+  <si>
+    <t>批量操作语句1执行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>批量操作语句2执行</t>
+  </si>
+  <si>
+    <t>csv_containsAll</t>
+  </si>
+  <si>
+    <t>batch_sql_01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_sql_02</t>
+  </si>
+  <si>
+    <t>Table_name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $batch01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_result1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_sql2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_result2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $batch02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Batch_sql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_sql1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_001.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_002.csv</t>
+  </si>
+  <si>
+    <t>batchsql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batchsql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_003</t>
+  </si>
+  <si>
+    <t>批量操作语句3执行</t>
+  </si>
+  <si>
+    <t>batch03</t>
+  </si>
+  <si>
+    <t>batch_sql_03</t>
+  </si>
+  <si>
+    <t>select * from $batch03</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_003.csv</t>
+  </si>
+  <si>
+    <t>batch_004</t>
+  </si>
+  <si>
+    <t>批量操作语句4执行</t>
+  </si>
+  <si>
+    <t>batch04</t>
+  </si>
+  <si>
+    <t>batch_sql_04</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_004.csv</t>
+  </si>
+  <si>
+    <t>select account from $batch04 where account&lt;&gt;'6225880178560985'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Testable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_005</t>
+  </si>
+  <si>
+    <t>批量操作语句5执行</t>
+  </si>
+  <si>
+    <t>batch05</t>
+  </si>
+  <si>
+    <t>batch_sql_05</t>
+  </si>
+  <si>
+    <t>select * from $batch05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_005.csv</t>
+  </si>
+  <si>
+    <t>batch_006</t>
+  </si>
+  <si>
+    <t>批量操作语句6执行</t>
+  </si>
+  <si>
+    <t>batch06</t>
+  </si>
+  <si>
+    <t>batch_sql_06</t>
+  </si>
+  <si>
+    <t>select * from $batch06</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_006.csv</t>
+  </si>
+  <si>
+    <t>batch_007</t>
+  </si>
+  <si>
+    <t>batch_008</t>
+  </si>
+  <si>
+    <t>批量操作语句7执行</t>
+  </si>
+  <si>
+    <t>批量操作语句8执行</t>
+  </si>
+  <si>
+    <t>batch07</t>
+  </si>
+  <si>
+    <t>batch08</t>
+  </si>
+  <si>
+    <t>batch_sql_07</t>
+  </si>
+  <si>
+    <t>batch_sql_08</t>
+  </si>
+  <si>
+    <t>select * from $batch07</t>
+  </si>
+  <si>
+    <t>select * from $batch08</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_007.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_008.csv</t>
+  </si>
+  <si>
+    <t>batch_009</t>
+  </si>
+  <si>
+    <t>批量操作语句9执行</t>
+  </si>
+  <si>
+    <t>batch_sql_09</t>
+  </si>
+  <si>
+    <t>select * from users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_009_01.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from roles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_009_02.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MultiTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>config_info,config_info_aggr,config_info_beta,config_info_tag,config_tags_relation,group_capacity,his_config_info,tenant_capacity,tenant_info,users,roles,permissions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Sub_component</t>
-  </si>
-  <si>
-    <t>Table_value_ref</t>
-  </si>
-  <si>
-    <t>Validation_type</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>csv_equals</t>
-  </si>
-  <si>
-    <t>批量操作语句1执行</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>批量操作语句2执行</t>
-  </si>
-  <si>
-    <t>csv_containsAll</t>
-  </si>
-  <si>
-    <t>batch_sql_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_sql_02</t>
-  </si>
-  <si>
-    <t>Table_name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from $batch01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_result1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_sql2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_result2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select * from $batch02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Batch_sql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_sql1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_001.csv</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_002.csv</t>
-  </si>
-  <si>
-    <t>batchsql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batchsql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_003</t>
-  </si>
-  <si>
-    <t>批量操作语句3执行</t>
-  </si>
-  <si>
-    <t>batch03</t>
-  </si>
-  <si>
-    <t>batch_sql_03</t>
-  </si>
-  <si>
-    <t>select * from $batch03</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_003.csv</t>
-  </si>
-  <si>
-    <t>batch_004</t>
-  </si>
-  <si>
-    <t>批量操作语句4执行</t>
-  </si>
-  <si>
-    <t>batch04</t>
-  </si>
-  <si>
-    <t>batch_sql_04</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_004.csv</t>
-  </si>
-  <si>
-    <t>select account from $batch04 where account&lt;&gt;'6225880178560985'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Testable</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_005</t>
-  </si>
-  <si>
-    <t>批量操作语句5执行</t>
-  </si>
-  <si>
-    <t>batch05</t>
-  </si>
-  <si>
-    <t>batch_sql_05</t>
-  </si>
-  <si>
-    <t>select * from $batch05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_005.csv</t>
-  </si>
-  <si>
-    <t>batch_006</t>
-  </si>
-  <si>
-    <t>批量操作语句6执行</t>
-  </si>
-  <si>
-    <t>batch06</t>
-  </si>
-  <si>
-    <t>batch_sql_06</t>
-  </si>
-  <si>
-    <t>select * from $batch06</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_006.csv</t>
-  </si>
-  <si>
-    <t>batch_007</t>
-  </si>
-  <si>
-    <t>batch_008</t>
-  </si>
-  <si>
-    <t>批量操作语句7执行</t>
-  </si>
-  <si>
-    <t>批量操作语句8执行</t>
-  </si>
-  <si>
-    <t>batch07</t>
-  </si>
-  <si>
-    <t>batch08</t>
-  </si>
-  <si>
-    <t>batch_sql_07</t>
-  </si>
-  <si>
-    <t>batch_sql_08</t>
-  </si>
-  <si>
-    <t>select * from $batch07</t>
-  </si>
-  <si>
-    <t>select * from $batch08</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_007.csv</t>
-  </si>
-  <si>
-    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_008.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SingleTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -606,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -633,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -642,263 +680,325 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="6" t="s">
+      <c r="H5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>39</v>
-      </c>
       <c r="M5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="M6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="6" t="s">
+      <c r="H7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>53</v>
-      </c>
       <c r="M7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>75</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J9" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="A10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>10</v>
+      <c r="B10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -908,7 +1008,7 @@
       <formula1>"y,n"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576">
-      <formula1>"csv_equals,csv_containsAll,string_equals,effected_rows_assert,assertNull,SQLException"</formula1>
+      <formula1>"csv_equals,csv_containsAll,string_equals,effected_rows_assert,assertNull,justExec,SQLException"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add case about jarvex and subquery
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
   <si>
     <t>TestID</t>
   </si>
@@ -271,6 +271,33 @@
   </si>
   <si>
     <t>SingleTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_010</t>
+  </si>
+  <si>
+    <t>批量操作语句10执行</t>
+  </si>
+  <si>
+    <t>batch_sql_10</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_010.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Schema</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JARVEX</t>
+  </si>
+  <si>
+    <t>JARVEX.CHAT_QU_DATA,JARVEX.CHAT_SE_DATA,JARVEX.COMMENT_BASE_INFO,JARVEX.CREATIVE_BASE_INFO,JARVEX.CREATIVE_QU_DATA,JARVEX.CREATIVE_SE_DATA,JARVEX.DATA_FILE,JARVEX.DATA_FILE_EXPERTISE,JARVEX.DATA_FILEFT,JARVEX.DATA_FILESET,JARVEX.DATA_FT_LIST,JARVEX.DATASET_DINGO,JARVEX.DATASET_FT_LIST,JARVEX.DEPARTMENT,JARVEX.MODEL_BASE_INFO,JARVEX.OPERATION,JARVEX.PERMISSION,JARVEX.PERMISSIONGROUP,JARVEX.REL_PGROUP_PERMISSION,JARVEX.REL_ROLE_PERMISSION,JARVEX.REL_ROLE_PGROUP,JARVEX.REL_USER_PERMISSION,JARVEX.REL_USER_ROLE,JARVEX.REL_USERGROUP_ROLE,JARVEX.REL_USERGROUP_USER,JARVEX.RESOURCE,JARVEX.ROLE,JARVEX.USER,JARVEX.USER_BASE,JARVEX.USERGROUP,JARVEX.VECTOR_DATA</t>
+  </si>
+  <si>
+    <t>select p.id pid, r.id rid, r.name rname, r.`type`, r.`key`, o.code, o.name oname, r.rel_id from JARVEX.PERMISSION as p left join JARVEX.RESOURCE as r on r.id = p.RESOURCE_ID and r.parent_id = 6 left join JARVEX.OPERATION as o on o.id = p.OPERATION_ID where r.id in (1, 3, 6, 8, 9, 21, 22, 23, 24, 33, 34, 35, 36, 37, 38, 39, 40, 66, 67, 68)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -644,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -657,16 +684,19 @@
     <col min="3" max="3" width="31.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="1" customWidth="1"/>
-    <col min="8" max="10" width="17.5" style="6" customWidth="1"/>
-    <col min="11" max="11" width="21.625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="19.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="1"/>
+    <col min="6" max="6" width="8.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" style="6" customWidth="1"/>
+    <col min="10" max="10" width="40.25" style="6" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="6" customWidth="1"/>
+    <col min="12" max="12" width="21.625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -682,32 +712,35 @@
       <c r="E1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>26</v>
       </c>
@@ -723,23 +756,23 @@
       <c r="E2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="I2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="K2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A3" s="6" t="s">
         <v>27</v>
       </c>
@@ -755,23 +788,23 @@
       <c r="E3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="K3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
         <v>28</v>
       </c>
@@ -787,23 +820,23 @@
       <c r="E4" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A5" s="6" t="s">
         <v>34</v>
       </c>
@@ -819,23 +852,23 @@
       <c r="E5" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="I5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
         <v>41</v>
       </c>
@@ -851,23 +884,23 @@
       <c r="E6" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="K6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" s="6" t="s">
         <v>47</v>
       </c>
@@ -883,23 +916,23 @@
       <c r="E7" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="K7" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="N7" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" s="6" t="s">
         <v>53</v>
       </c>
@@ -915,23 +948,23 @@
       <c r="E8" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="K8" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="M8" s="6" t="s">
+      <c r="N8" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" s="6" t="s">
         <v>54</v>
       </c>
@@ -947,23 +980,23 @@
       <c r="E9" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="I9" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="K9" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="M9" s="6" t="s">
+      <c r="N9" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" s="6" t="s">
         <v>65</v>
       </c>
@@ -979,25 +1012,60 @@
       <c r="E10" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="I10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="J10" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="K10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K10" s="6" t="s">
+      <c r="L10" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="L10" s="8" t="s">
+      <c r="M10" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1007,7 +1075,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>"y,n"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N1048576">
       <formula1>"csv_equals,csv_containsAll,string_equals,effected_rows_assert,assertNull,justExec,SQLException"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add case about auto_increment refresh and json \r\n escape
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
   <si>
     <t>TestID</t>
   </si>
@@ -299,6 +299,26 @@
   <si>
     <t>select p.id pid, r.id rid, r.name rname, r.`type`, r.`key`, o.code, o.name oname, r.rel_id from JARVEX.PERMISSION as p left join JARVEX.RESOURCE as r on r.id = p.RESOURCE_ID and r.parent_id = 6 left join JARVEX.OPERATION as o on o.id = p.OPERATION_ID where r.id in (1, 3, 6, 8, 9, 21, 22, 23, 24, 33, 34, 35, 36, 37, 38, 39, 40, 66, 67, 68)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_011</t>
+  </si>
+  <si>
+    <t>批量操作语句11执行</t>
+  </si>
+  <si>
+    <t>batch11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_sql_11</t>
+  </si>
+  <si>
+    <t>select * from $batch11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_011.csv</t>
   </si>
 </sst>
 </file>
@@ -671,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1066,6 +1086,38 @@
         <v>79</v>
       </c>
       <c r="N11" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A12" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add one more case about auto_increment
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
   <si>
     <t>TestID</t>
   </si>
@@ -280,9 +280,6 @@
     <t>批量操作语句10执行</t>
   </si>
   <si>
-    <t>batch_sql_10</t>
-  </si>
-  <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_010.csv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -307,18 +304,44 @@
     <t>批量操作语句11执行</t>
   </si>
   <si>
-    <t>batch11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>batch_sql_11</t>
-  </si>
-  <si>
-    <t>select * from $batch11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_011.csv</t>
+  </si>
+  <si>
+    <t>batch_012</t>
+  </si>
+  <si>
+    <t>批量操作语句12执行</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_012.csv</t>
+  </si>
+  <si>
+    <t>batch011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $batch011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $batch012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_sql_010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_sql_011</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_sql_012</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -691,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -733,7 +756,7 @@
         <v>74</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>12</v>
@@ -1068,22 +1091,22 @@
         <v>24</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="I11" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="K11" s="8" t="s">
         <v>78</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="N11" s="6" t="s">
         <v>9</v>
@@ -1091,13 +1114,13 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>24</v>
@@ -1106,18 +1129,50 @@
         <v>75</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="B13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="D13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="K12" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="N13" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add cases about BTREE engine
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="114">
   <si>
     <t>TestID</t>
   </si>
@@ -342,6 +342,62 @@
   <si>
     <t>batch_sql_012</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_013</t>
+  </si>
+  <si>
+    <t>批量操作语句13执行</t>
+  </si>
+  <si>
+    <t>batch013</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_sql_013</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_013.csv</t>
+  </si>
+  <si>
+    <t>batch_014</t>
+  </si>
+  <si>
+    <t>批量操作语句14执行</t>
+  </si>
+  <si>
+    <t>batch014</t>
+  </si>
+  <si>
+    <t>batch_sql_014</t>
+  </si>
+  <si>
+    <t>select * from $batch013</t>
+  </si>
+  <si>
+    <t>select * from $batch014</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_014.csv</t>
+  </si>
+  <si>
+    <t>batch_015</t>
+  </si>
+  <si>
+    <t>批量操作语句15执行</t>
+  </si>
+  <si>
+    <t>batch015</t>
+  </si>
+  <si>
+    <t>batch_sql_015</t>
+  </si>
+  <si>
+    <t>select id,name,age from $batch015</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_015.csv</t>
   </si>
 </sst>
 </file>
@@ -714,10 +770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1173,6 +1229,102 @@
         <v>88</v>
       </c>
       <c r="N13" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A15" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N16" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
open Dingo dataprovider parallel
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/batchsql/sql_batchsql_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="120">
   <si>
     <t>TestID</t>
   </si>
@@ -398,6 +398,26 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_015.csv</t>
+  </si>
+  <si>
+    <t>batch_016</t>
+  </si>
+  <si>
+    <t>批量操作语句16执行</t>
+  </si>
+  <si>
+    <t>v</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>batch_sql_016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select a.id from v as a </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/batchsql/expectedresult/batch_016.csv</t>
   </si>
 </sst>
 </file>
@@ -770,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1325,6 +1345,38 @@
         <v>113</v>
       </c>
       <c r="N16" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A17" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="N17" s="1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>